<commit_message>
Generate Student EDA Signed-off-by: Alejandro <alejandro.adrian@exponentiateam.com>
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/EdRecord.xlsx
+++ b/spec/fixtures/files/EdRecord.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\workspace\eschooltul\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alejandro\workspace\eschooltul_backend\spec\fixtures\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C7B0AB-694D-4E99-9F6D-75A2036B7CC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6596BC57-992A-4729-9202-A271E249B846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4620" yWindow="-21720" windowWidth="38640" windowHeight="21240" xr2:uid="{23991A37-0B98-475E-8FF7-AA44DB67095C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{23991A37-0B98-475E-8FF7-AA44DB67095C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -39,9 +39,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Age</t>
-  </si>
-  <si>
     <t>First_surname</t>
   </si>
   <si>
@@ -79,6 +76,9 @@
   </si>
   <si>
     <t>Simpson</t>
+  </si>
+  <si>
+    <t>Birthday</t>
   </si>
 </sst>
 </file>
@@ -114,8 +114,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,84 +434,84 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="12.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
+      <c r="B2" s="1">
+        <v>29221</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1">
+        <v>29221</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="B2">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B3">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
+      <c r="B4" s="1">
+        <v>29221</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="B5" s="1">
+        <v>29221</v>
+      </c>
+      <c r="C5" t="s">
         <v>13</v>
-      </c>
-      <c r="B5">
-        <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>